<commit_message>
nike and adidas youth products added to categories
There are different vendor codes for youth products form these two
brands. These extra vendor codes have been added to their respective
"main" brand categories so that they will show in results for those
categories.
</commit_message>
<xml_diff>
--- a/filters/db/Brands.xlsx
+++ b/filters/db/Brands.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="375" windowWidth="19875" windowHeight="8235"/>
+    <workbookView xWindow="360" yWindow="375" windowWidth="19875" windowHeight="8235" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Brands" sheetId="1" r:id="rId1"/>
+    <sheet name="Special Circumstances" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="206">
   <si>
     <t>id</t>
   </si>
@@ -629,6 +630,9 @@
   </si>
   <si>
     <t>Tervis</t>
+  </si>
+  <si>
+    <t>1. Adidas and Nike both have youth vendor codes: yadds &amp; nike-y that need to be added to the json until the json building utility is set to read mulitple attributes</t>
   </si>
 </sst>
 </file>
@@ -672,10 +676,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -979,7 +986,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A79" sqref="A79"/>
     </sheetView>
   </sheetViews>
@@ -3266,4 +3273,31 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="113.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="284.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
47 Brand fix / version
The single quote at the beginning of the 47 Brand id was breaking the
search for the category.
Also moved the other two vendor id's that were present for this brand
into an OR in a single page and removed the other page occurrences.
</commit_message>
<xml_diff>
--- a/filters/db/Brands.xlsx
+++ b/filters/db/Brands.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="208">
   <si>
     <t>id</t>
   </si>
@@ -632,7 +632,13 @@
     <t>Tervis</t>
   </si>
   <si>
-    <t>1. Adidas and Nike both have youth vendor codes: yadds &amp; nike-y that need to be added to the json until the json building utility is set to read mulitple attributes</t>
+    <t>47 Brand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The id for 47 Brand includes a singe quote: '47 Brand. This breaks elastic for this category, so remove it if the data is re-populated in the future. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Several vendors have multiple codes. Until these can be accounted for in the utility they have been consolodated by hand in the json.  These vendors include (but may not be limited to): Nike, Adidas, 47 Brand. </t>
   </si>
 </sst>
 </file>
@@ -676,12 +682,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -987,7 +996,7 @@
   <dimension ref="A1:G99"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A79" sqref="A79"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1201,7 +1210,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>205</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
@@ -3277,7 +3286,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -3286,14 +3295,14 @@
     <col min="1" max="1" width="113.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="284.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
+        <v>207</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>206</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update brands json w/ multiple codes / version
New brands were added, and several on both the new and old set had
multiple vendor codes.
The a category object for each code was being generated resulting in
different categories w/ the same name and link.
Created an OR in the base filter for each of these categories so
products for both codes would show in a single category for that
brand/vendor.
The json generator will need to be altered to do this automatically.
</commit_message>
<xml_diff>
--- a/filters/db/Brands.xlsx
+++ b/filters/db/Brands.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="766" uniqueCount="247">
   <si>
     <t>id</t>
   </si>
@@ -41,9 +41,6 @@
     <t>Shop Campus Colors for thousands of NCAA, NFL, NBA, MLB, &amp; NHL products, novelties and more! We offer gear from top brands such as Nike &amp; Adidas. Ship Same-Day to All 50 States!</t>
   </si>
   <si>
-    <t>banners/test_cat_banner_785x200.jpg</t>
-  </si>
-  <si>
     <t>Some promotional text goes here</t>
   </si>
   <si>
@@ -113,9 +110,6 @@
     <t>Comfy Feet</t>
   </si>
   <si>
-    <t>Colossuem</t>
-  </si>
-  <si>
     <t>Concept One</t>
   </si>
   <si>
@@ -632,13 +626,136 @@
     <t>Tervis</t>
   </si>
   <si>
-    <t>47 Brand</t>
-  </si>
-  <si>
     <t xml:space="preserve">The id for 47 Brand includes a singe quote: '47 Brand. This breaks elastic for this category, so remove it if the data is re-populated in the future. </t>
   </si>
   <si>
-    <t xml:space="preserve">Several vendors have multiple codes. Until these can be accounted for in the utility they have been consolodated by hand in the json.  These vendors include (but may not be limited to): Nike, Adidas, 47 Brand. </t>
+    <t>All-Sportz Brush</t>
+  </si>
+  <si>
+    <t>Colosseum</t>
+  </si>
+  <si>
+    <t>Dallas Cowboys Merchandise</t>
+  </si>
+  <si>
+    <t>Duck House Sports</t>
+  </si>
+  <si>
+    <t>Elite Image Eyewear</t>
+  </si>
+  <si>
+    <t>Gameday Spirit</t>
+  </si>
+  <si>
+    <t>Glitter Girl</t>
+  </si>
+  <si>
+    <t>League Collegiate Outfitters</t>
+  </si>
+  <si>
+    <t>Mascot Factory</t>
+  </si>
+  <si>
+    <t>Me &amp; My Big Ideas</t>
+  </si>
+  <si>
+    <t>MV Sport</t>
+  </si>
+  <si>
+    <t>Pinemeadow Green</t>
+  </si>
+  <si>
+    <t>Sutter's Mill</t>
+  </si>
+  <si>
+    <t>Team Sports America</t>
+  </si>
+  <si>
+    <t>P-TWN</t>
+  </si>
+  <si>
+    <t>ASB</t>
+  </si>
+  <si>
+    <t>P-AMIN</t>
+  </si>
+  <si>
+    <t>P-BSI</t>
+  </si>
+  <si>
+    <t>P-CONE</t>
+  </si>
+  <si>
+    <t>P-DCM</t>
+  </si>
+  <si>
+    <t>P-DHS</t>
+  </si>
+  <si>
+    <t>EIE</t>
+  </si>
+  <si>
+    <t>P-FBF</t>
+  </si>
+  <si>
+    <t>GS</t>
+  </si>
+  <si>
+    <t>GLIT</t>
+  </si>
+  <si>
+    <t>P-HUN</t>
+  </si>
+  <si>
+    <t>LCO</t>
+  </si>
+  <si>
+    <t>P-MAJ</t>
+  </si>
+  <si>
+    <t>MAS</t>
+  </si>
+  <si>
+    <t>MMBI</t>
+  </si>
+  <si>
+    <t>MV</t>
+  </si>
+  <si>
+    <t>P-NE</t>
+  </si>
+  <si>
+    <t>PINE</t>
+  </si>
+  <si>
+    <t>P-RICO</t>
+  </si>
+  <si>
+    <t>P-RID</t>
+  </si>
+  <si>
+    <t>SUT</t>
+  </si>
+  <si>
+    <t>P-TSA</t>
+  </si>
+  <si>
+    <t>P-NW</t>
+  </si>
+  <si>
+    <t>P-TOP</t>
+  </si>
+  <si>
+    <t>P-MCAR</t>
+  </si>
+  <si>
+    <t>P-WIN</t>
+  </si>
+  <si>
+    <t>P-WSS</t>
+  </si>
+  <si>
+    <t>Several vendors have multiple codes. Until these can be accounted for in the utility they have been consolodated by hand in the json.  These vendors include (but may not be limited to): '47 Brand, Adidas, Aminco, BSI Products, Campus Colors, Concept One, For Bare Feet, Highland Mint, Hunter, Majestic, New Era, Nike, Reebok, Rico, Ridell, The Northwest, Topperscot, Wincraft, Winning Streak Sports.</t>
   </si>
 </sst>
 </file>
@@ -993,10 +1110,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G99"/>
+  <dimension ref="A1:G127"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView topLeftCell="A101" workbookViewId="0">
+      <selection activeCell="A124" sqref="A124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1029,65 +1146,65 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
         <v>17</v>
       </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="G2" t="s">
         <v>8</v>
-      </c>
-      <c r="F2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="F4" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="G4">
         <v>150</v>
@@ -1095,22 +1212,22 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>107</v>
+        <v>218</v>
       </c>
       <c r="F5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G5">
         <v>150</v>
@@ -1118,22 +1235,22 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E6" t="s">
-        <v>108</v>
+        <v>188</v>
       </c>
       <c r="F6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G6">
         <v>150</v>
@@ -1141,22 +1258,22 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E7" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="F7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G7">
         <v>150</v>
@@ -1164,22 +1281,22 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E8" t="s">
-        <v>110</v>
+        <v>194</v>
       </c>
       <c r="F8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G8">
         <v>150</v>
@@ -1187,22 +1304,22 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>204</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E9" t="s">
-        <v>111</v>
+        <v>219</v>
       </c>
       <c r="F9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G9">
         <v>150</v>
@@ -1210,22 +1327,22 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>205</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E10" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="F10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G10">
         <v>150</v>
@@ -1233,22 +1350,22 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B11" t="s">
         <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E11" t="s">
-        <v>113</v>
+        <v>220</v>
       </c>
       <c r="F11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G11">
         <v>150</v>
@@ -1256,22 +1373,22 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B12" t="s">
         <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E12" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="F12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G12">
         <v>150</v>
@@ -1279,22 +1396,22 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B13" t="s">
         <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E13" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="F13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G13">
         <v>150</v>
@@ -1302,22 +1419,22 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B14" t="s">
         <v>7</v>
       </c>
       <c r="C14" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E14" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="F14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G14">
         <v>150</v>
@@ -1325,22 +1442,22 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B15" t="s">
         <v>7</v>
       </c>
       <c r="C15" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E15" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="F15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G15">
         <v>150</v>
@@ -1348,22 +1465,22 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B16" t="s">
         <v>7</v>
       </c>
       <c r="C16" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E16" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="F16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G16">
         <v>150</v>
@@ -1371,22 +1488,22 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B17" t="s">
         <v>7</v>
       </c>
       <c r="C17" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E17" t="s">
-        <v>119</v>
+        <v>221</v>
       </c>
       <c r="F17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G17">
         <v>150</v>
@@ -1394,22 +1511,22 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B18" t="s">
         <v>7</v>
       </c>
       <c r="C18" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E18" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="F18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G18">
         <v>150</v>
@@ -1417,22 +1534,22 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>34</v>
+        <v>62</v>
       </c>
       <c r="B19" t="s">
         <v>7</v>
       </c>
       <c r="C19" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E19" t="s">
-        <v>121</v>
+        <v>149</v>
       </c>
       <c r="F19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G19">
         <v>150</v>
@@ -1440,22 +1557,22 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>35</v>
+        <v>62</v>
       </c>
       <c r="B20" t="s">
         <v>7</v>
       </c>
       <c r="C20" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E20" t="s">
-        <v>122</v>
+        <v>190</v>
       </c>
       <c r="F20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G20">
         <v>150</v>
@@ -1463,22 +1580,22 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B21" t="s">
         <v>7</v>
       </c>
       <c r="C21" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E21" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="F21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G21">
         <v>150</v>
@@ -1486,22 +1603,22 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="B22" t="s">
         <v>7</v>
       </c>
       <c r="C22" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E22" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="F22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G22">
         <v>150</v>
@@ -1509,22 +1626,22 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>38</v>
+        <v>205</v>
       </c>
       <c r="B23" t="s">
         <v>7</v>
       </c>
       <c r="C23" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D23" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E23" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="F23" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G23">
         <v>150</v>
@@ -1532,22 +1649,22 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B24" t="s">
         <v>7</v>
       </c>
       <c r="C24" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E24" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="F24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G24">
         <v>150</v>
@@ -1555,22 +1672,22 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="B25" t="s">
         <v>7</v>
       </c>
       <c r="C25" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E25" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="F25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G25">
         <v>150</v>
@@ -1578,22 +1695,22 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="B26" t="s">
         <v>7</v>
       </c>
       <c r="C26" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D26" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E26" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="F26" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G26">
         <v>150</v>
@@ -1601,22 +1718,22 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="B27" t="s">
         <v>7</v>
       </c>
       <c r="C27" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D27" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E27" t="s">
-        <v>129</v>
+        <v>222</v>
       </c>
       <c r="F27" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G27">
         <v>150</v>
@@ -1624,22 +1741,22 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="B28" t="s">
         <v>7</v>
       </c>
       <c r="C28" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D28" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E28" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="F28" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G28">
         <v>150</v>
@@ -1647,22 +1764,22 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="B29" t="s">
         <v>7</v>
       </c>
       <c r="C29" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D29" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E29" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="F29" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G29">
         <v>150</v>
@@ -1670,22 +1787,22 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>45</v>
+        <v>206</v>
       </c>
       <c r="B30" t="s">
         <v>7</v>
       </c>
       <c r="C30" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E30" t="s">
-        <v>132</v>
+        <v>223</v>
       </c>
       <c r="F30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G30">
         <v>150</v>
@@ -1693,22 +1810,22 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="B31" t="s">
         <v>7</v>
       </c>
       <c r="C31" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D31" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E31" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="F31" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G31">
         <v>150</v>
@@ -1716,22 +1833,22 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>47</v>
+        <v>207</v>
       </c>
       <c r="B32" t="s">
         <v>7</v>
       </c>
       <c r="C32" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D32" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E32" t="s">
-        <v>134</v>
+        <v>224</v>
       </c>
       <c r="F32" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G32">
         <v>150</v>
@@ -1739,22 +1856,22 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>48</v>
+        <v>208</v>
       </c>
       <c r="B33" t="s">
         <v>7</v>
       </c>
       <c r="C33" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D33" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E33" t="s">
-        <v>135</v>
+        <v>225</v>
       </c>
       <c r="F33" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G33">
         <v>150</v>
@@ -1762,22 +1879,22 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>49</v>
+        <v>88</v>
       </c>
       <c r="B34" t="s">
         <v>7</v>
       </c>
       <c r="C34" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D34" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E34" t="s">
-        <v>136</v>
+        <v>176</v>
       </c>
       <c r="F34" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G34">
         <v>150</v>
@@ -1785,22 +1902,22 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="B35" t="s">
         <v>7</v>
       </c>
       <c r="C35" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D35" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E35" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="F35" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G35">
         <v>150</v>
@@ -1808,22 +1925,22 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B36" t="s">
         <v>7</v>
       </c>
       <c r="C36" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D36" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E36" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="F36" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G36">
         <v>150</v>
@@ -1831,22 +1948,22 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="B37" t="s">
         <v>7</v>
       </c>
       <c r="C37" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D37" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E37" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="F37" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G37">
         <v>150</v>
@@ -1854,22 +1971,22 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="B38" t="s">
         <v>7</v>
       </c>
       <c r="C38" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D38" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E38" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="F38" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G38">
         <v>150</v>
@@ -1877,22 +1994,22 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="B39" t="s">
         <v>7</v>
       </c>
       <c r="C39" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D39" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E39" t="s">
-        <v>141</v>
+        <v>122</v>
       </c>
       <c r="F39" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G39">
         <v>150</v>
@@ -1900,22 +2017,22 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="B40" t="s">
         <v>7</v>
       </c>
       <c r="C40" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D40" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E40" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F40" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G40">
         <v>150</v>
@@ -1923,22 +2040,22 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="B41" t="s">
         <v>7</v>
       </c>
       <c r="C41" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D41" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E41" t="s">
-        <v>143</v>
+        <v>125</v>
       </c>
       <c r="F41" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G41">
         <v>150</v>
@@ -1946,22 +2063,22 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>57</v>
+        <v>38</v>
       </c>
       <c r="B42" t="s">
         <v>7</v>
       </c>
       <c r="C42" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D42" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E42" t="s">
-        <v>144</v>
+        <v>226</v>
       </c>
       <c r="F42" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G42">
         <v>150</v>
@@ -1969,22 +2086,22 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="B43" t="s">
         <v>7</v>
       </c>
       <c r="C43" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D43" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E43" t="s">
-        <v>145</v>
+        <v>130</v>
       </c>
       <c r="F43" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G43">
         <v>150</v>
@@ -1992,22 +2109,22 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="B44" t="s">
         <v>7</v>
       </c>
       <c r="C44" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D44" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E44" t="s">
-        <v>146</v>
+        <v>128</v>
       </c>
       <c r="F44" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G44">
         <v>150</v>
@@ -2015,22 +2132,22 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="B45" t="s">
         <v>7</v>
       </c>
       <c r="C45" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D45" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E45" t="s">
-        <v>147</v>
+        <v>129</v>
       </c>
       <c r="F45" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G45">
         <v>150</v>
@@ -2038,22 +2155,22 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="B46" t="s">
         <v>7</v>
       </c>
       <c r="C46" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D46" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E46" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="F46" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G46">
         <v>150</v>
@@ -2061,22 +2178,22 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>62</v>
+        <v>209</v>
       </c>
       <c r="B47" t="s">
         <v>7</v>
       </c>
       <c r="C47" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D47" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E47" t="s">
-        <v>149</v>
+        <v>227</v>
       </c>
       <c r="F47" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G47">
         <v>150</v>
@@ -2084,22 +2201,22 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="B48" t="s">
         <v>7</v>
       </c>
       <c r="C48" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D48" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E48" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
       <c r="F48" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G48">
         <v>150</v>
@@ -2107,22 +2224,22 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B49" t="s">
         <v>7</v>
       </c>
       <c r="C49" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D49" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E49" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="F49" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G49">
         <v>150</v>
@@ -2130,22 +2247,22 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="B50" t="s">
         <v>7</v>
       </c>
       <c r="C50" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D50" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E50" t="s">
-        <v>152</v>
+        <v>136</v>
       </c>
       <c r="F50" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G50">
         <v>150</v>
@@ -2153,22 +2270,22 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>66</v>
+        <v>210</v>
       </c>
       <c r="B51" t="s">
         <v>7</v>
       </c>
       <c r="C51" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D51" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E51" t="s">
-        <v>153</v>
+        <v>228</v>
       </c>
       <c r="F51" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G51">
         <v>150</v>
@@ -2176,22 +2293,22 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="B52" t="s">
         <v>7</v>
       </c>
       <c r="C52" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D52" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E52" t="s">
-        <v>154</v>
+        <v>135</v>
       </c>
       <c r="F52" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G52">
         <v>150</v>
@@ -2199,22 +2316,22 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>67</v>
+        <v>46</v>
       </c>
       <c r="B53" t="s">
         <v>7</v>
       </c>
       <c r="C53" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D53" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E53" t="s">
-        <v>155</v>
+        <v>133</v>
       </c>
       <c r="F53" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G53">
         <v>150</v>
@@ -2222,22 +2339,22 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="B54" t="s">
         <v>7</v>
       </c>
       <c r="C54" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D54" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E54" t="s">
-        <v>156</v>
+        <v>138</v>
       </c>
       <c r="F54" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G54">
         <v>150</v>
@@ -2245,22 +2362,22 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="B55" t="s">
         <v>7</v>
       </c>
       <c r="C55" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D55" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E55" t="s">
-        <v>157</v>
+        <v>182</v>
       </c>
       <c r="F55" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G55">
         <v>150</v>
@@ -2268,22 +2385,22 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="B56" t="s">
         <v>7</v>
       </c>
       <c r="C56" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D56" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E56" t="s">
-        <v>158</v>
+        <v>139</v>
       </c>
       <c r="F56" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G56">
         <v>150</v>
@@ -2291,22 +2408,22 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="B57" t="s">
         <v>7</v>
       </c>
       <c r="C57" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D57" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E57" t="s">
-        <v>159</v>
+        <v>140</v>
       </c>
       <c r="F57" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G57">
         <v>150</v>
@@ -2314,22 +2431,22 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>72</v>
+        <v>53</v>
       </c>
       <c r="B58" t="s">
         <v>7</v>
       </c>
       <c r="C58" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D58" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E58" t="s">
-        <v>160</v>
+        <v>229</v>
       </c>
       <c r="F58" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G58">
         <v>150</v>
@@ -2337,22 +2454,22 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>73</v>
+        <v>54</v>
       </c>
       <c r="B59" t="s">
         <v>7</v>
       </c>
       <c r="C59" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D59" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E59" t="s">
-        <v>161</v>
+        <v>141</v>
       </c>
       <c r="F59" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G59">
         <v>150</v>
@@ -2360,22 +2477,22 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>74</v>
+        <v>55</v>
       </c>
       <c r="B60" t="s">
         <v>7</v>
       </c>
       <c r="C60" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D60" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E60" t="s">
-        <v>162</v>
+        <v>142</v>
       </c>
       <c r="F60" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G60">
         <v>150</v>
@@ -2383,22 +2500,22 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="B61" t="s">
         <v>7</v>
       </c>
       <c r="C61" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D61" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E61" t="s">
-        <v>163</v>
+        <v>144</v>
       </c>
       <c r="F61" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G61">
         <v>150</v>
@@ -2406,22 +2523,22 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>76</v>
+        <v>211</v>
       </c>
       <c r="B62" t="s">
         <v>7</v>
       </c>
       <c r="C62" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D62" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E62" t="s">
-        <v>164</v>
+        <v>230</v>
       </c>
       <c r="F62" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G62">
         <v>150</v>
@@ -2429,22 +2546,22 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="B63" t="s">
         <v>7</v>
       </c>
       <c r="C63" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D63" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E63" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="F63" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G63">
         <v>150</v>
@@ -2452,22 +2569,22 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="B64" t="s">
         <v>7</v>
       </c>
       <c r="C64" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D64" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E64" t="s">
-        <v>166</v>
+        <v>145</v>
       </c>
       <c r="F64" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G64">
         <v>150</v>
@@ -2475,22 +2592,22 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>79</v>
+        <v>59</v>
       </c>
       <c r="B65" t="s">
         <v>7</v>
       </c>
       <c r="C65" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D65" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E65" t="s">
-        <v>167</v>
+        <v>146</v>
       </c>
       <c r="F65" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G65">
         <v>150</v>
@@ -2498,22 +2615,22 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="B66" t="s">
         <v>7</v>
       </c>
       <c r="C66" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D66" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E66" t="s">
-        <v>168</v>
+        <v>147</v>
       </c>
       <c r="F66" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G66">
         <v>150</v>
@@ -2521,22 +2638,22 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="B67" t="s">
         <v>7</v>
       </c>
       <c r="C67" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D67" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E67" t="s">
-        <v>169</v>
+        <v>231</v>
       </c>
       <c r="F67" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G67">
         <v>150</v>
@@ -2544,22 +2661,22 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>82</v>
+        <v>60</v>
       </c>
       <c r="B68" t="s">
         <v>7</v>
       </c>
       <c r="C68" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D68" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E68" t="s">
-        <v>170</v>
+        <v>195</v>
       </c>
       <c r="F68" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G68">
         <v>150</v>
@@ -2567,22 +2684,22 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>83</v>
+        <v>212</v>
       </c>
       <c r="B69" t="s">
         <v>7</v>
       </c>
       <c r="C69" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D69" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E69" t="s">
-        <v>171</v>
+        <v>232</v>
       </c>
       <c r="F69" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G69">
         <v>150</v>
@@ -2590,22 +2707,22 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>84</v>
+        <v>213</v>
       </c>
       <c r="B70" t="s">
         <v>7</v>
       </c>
       <c r="C70" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D70" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E70" t="s">
-        <v>172</v>
+        <v>233</v>
       </c>
       <c r="F70" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G70">
         <v>150</v>
@@ -2613,22 +2730,22 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="B71" t="s">
         <v>7</v>
       </c>
       <c r="C71" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D71" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E71" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="F71" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G71">
         <v>150</v>
@@ -2636,22 +2753,22 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>86</v>
+        <v>214</v>
       </c>
       <c r="B72" t="s">
         <v>7</v>
       </c>
       <c r="C72" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D72" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E72" t="s">
-        <v>174</v>
+        <v>234</v>
       </c>
       <c r="F72" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G72">
         <v>150</v>
@@ -2659,22 +2776,22 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>87</v>
+        <v>63</v>
       </c>
       <c r="B73" t="s">
         <v>7</v>
       </c>
       <c r="C73" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D73" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E73" t="s">
-        <v>175</v>
+        <v>150</v>
       </c>
       <c r="F73" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G73">
         <v>150</v>
@@ -2682,22 +2799,22 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>88</v>
+        <v>63</v>
       </c>
       <c r="B74" t="s">
         <v>7</v>
       </c>
       <c r="C74" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D74" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E74" t="s">
-        <v>176</v>
+        <v>235</v>
       </c>
       <c r="F74" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G74">
         <v>150</v>
@@ -2705,22 +2822,22 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="B75" t="s">
         <v>7</v>
       </c>
       <c r="C75" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D75" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E75" t="s">
-        <v>177</v>
+        <v>196</v>
       </c>
       <c r="F75" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G75">
         <v>150</v>
@@ -2728,22 +2845,22 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>90</v>
+        <v>64</v>
       </c>
       <c r="B76" t="s">
         <v>7</v>
       </c>
       <c r="C76" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D76" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E76" t="s">
-        <v>178</v>
+        <v>151</v>
       </c>
       <c r="F76" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G76">
         <v>150</v>
@@ -2751,22 +2868,22 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>91</v>
+        <v>64</v>
       </c>
       <c r="B77" t="s">
         <v>7</v>
       </c>
       <c r="C77" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D77" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E77" t="s">
-        <v>179</v>
+        <v>152</v>
       </c>
       <c r="F77" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G77">
         <v>150</v>
@@ -2774,22 +2891,22 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="B78" t="s">
         <v>7</v>
       </c>
       <c r="C78" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D78" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E78" t="s">
-        <v>180</v>
+        <v>162</v>
       </c>
       <c r="F78" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G78">
         <v>150</v>
@@ -2797,22 +2914,22 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>204</v>
+        <v>67</v>
       </c>
       <c r="B79" t="s">
         <v>7</v>
       </c>
       <c r="C79" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D79" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E79" t="s">
-        <v>181</v>
+        <v>155</v>
       </c>
       <c r="F79" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G79">
         <v>150</v>
@@ -2820,22 +2937,22 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>93</v>
+        <v>69</v>
       </c>
       <c r="B80" t="s">
         <v>7</v>
       </c>
       <c r="C80" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D80" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E80" t="s">
-        <v>182</v>
+        <v>157</v>
       </c>
       <c r="F80" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G80">
         <v>150</v>
@@ -2843,22 +2960,22 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>94</v>
+        <v>215</v>
       </c>
       <c r="B81" t="s">
         <v>7</v>
       </c>
       <c r="C81" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D81" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E81" t="s">
-        <v>183</v>
+        <v>236</v>
       </c>
       <c r="F81" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G81">
         <v>150</v>
@@ -2866,22 +2983,22 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
       <c r="B82" t="s">
         <v>7</v>
       </c>
       <c r="C82" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D82" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E82" t="s">
-        <v>184</v>
+        <v>158</v>
       </c>
       <c r="F82" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G82">
         <v>150</v>
@@ -2889,22 +3006,22 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>95</v>
+        <v>72</v>
       </c>
       <c r="B83" t="s">
         <v>7</v>
       </c>
       <c r="C83" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D83" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E83" t="s">
-        <v>185</v>
+        <v>160</v>
       </c>
       <c r="F83" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G83">
         <v>150</v>
@@ -2912,22 +3029,22 @@
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>96</v>
+        <v>73</v>
       </c>
       <c r="B84" t="s">
         <v>7</v>
       </c>
       <c r="C84" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D84" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E84" t="s">
-        <v>186</v>
+        <v>161</v>
       </c>
       <c r="F84" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G84">
         <v>150</v>
@@ -2935,22 +3052,22 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="B85" t="s">
         <v>7</v>
       </c>
       <c r="C85" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D85" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E85" t="s">
-        <v>187</v>
+        <v>167</v>
       </c>
       <c r="F85" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G85">
         <v>150</v>
@@ -2958,22 +3075,22 @@
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>98</v>
+        <v>56</v>
       </c>
       <c r="B86" t="s">
         <v>7</v>
       </c>
       <c r="C86" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D86" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E86" t="s">
-        <v>188</v>
+        <v>143</v>
       </c>
       <c r="F86" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G86">
         <v>150</v>
@@ -2981,22 +3098,22 @@
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>99</v>
+        <v>75</v>
       </c>
       <c r="B87" t="s">
         <v>7</v>
       </c>
       <c r="C87" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D87" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E87" t="s">
-        <v>189</v>
+        <v>163</v>
       </c>
       <c r="F87" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G87">
         <v>150</v>
@@ -3004,22 +3121,22 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="B88" t="s">
         <v>7</v>
       </c>
       <c r="C88" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D88" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E88" t="s">
-        <v>190</v>
+        <v>197</v>
       </c>
       <c r="F88" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G88">
         <v>150</v>
@@ -3027,22 +3144,22 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>100</v>
+        <v>77</v>
       </c>
       <c r="B89" t="s">
         <v>7</v>
       </c>
       <c r="C89" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D89" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E89" t="s">
-        <v>191</v>
+        <v>237</v>
       </c>
       <c r="F89" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G89">
         <v>150</v>
@@ -3050,22 +3167,22 @@
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="B90" t="s">
         <v>7</v>
       </c>
       <c r="C90" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D90" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E90" t="s">
-        <v>192</v>
+        <v>165</v>
       </c>
       <c r="F90" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G90">
         <v>150</v>
@@ -3073,22 +3190,22 @@
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="B91" t="s">
         <v>7</v>
       </c>
       <c r="C91" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D91" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E91" t="s">
-        <v>193</v>
+        <v>238</v>
       </c>
       <c r="F91" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G91">
         <v>150</v>
@@ -3096,22 +3213,22 @@
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>101</v>
+        <v>78</v>
       </c>
       <c r="B92" t="s">
         <v>7</v>
       </c>
       <c r="C92" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D92" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E92" t="s">
-        <v>194</v>
+        <v>166</v>
       </c>
       <c r="F92" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G92">
         <v>150</v>
@@ -3119,22 +3236,22 @@
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="B93" t="s">
         <v>7</v>
       </c>
       <c r="C93" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D93" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E93" t="s">
-        <v>195</v>
+        <v>168</v>
       </c>
       <c r="F93" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G93">
         <v>150</v>
@@ -3142,22 +3259,22 @@
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="B94" t="s">
         <v>7</v>
       </c>
       <c r="C94" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D94" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E94" t="s">
-        <v>196</v>
+        <v>169</v>
       </c>
       <c r="F94" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G94">
         <v>150</v>
@@ -3165,22 +3282,22 @@
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>62</v>
+        <v>83</v>
       </c>
       <c r="B95" t="s">
         <v>7</v>
       </c>
       <c r="C95" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D95" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E95" t="s">
-        <v>197</v>
+        <v>171</v>
       </c>
       <c r="F95" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G95">
         <v>150</v>
@@ -3188,22 +3305,22 @@
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>103</v>
+        <v>82</v>
       </c>
       <c r="B96" t="s">
         <v>7</v>
       </c>
       <c r="C96" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D96" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E96" t="s">
-        <v>198</v>
+        <v>170</v>
       </c>
       <c r="F96" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G96">
         <v>150</v>
@@ -3211,22 +3328,22 @@
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="B97" t="s">
         <v>7</v>
       </c>
       <c r="C97" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D97" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E97" t="s">
-        <v>199</v>
+        <v>172</v>
       </c>
       <c r="F97" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G97">
         <v>150</v>
@@ -3234,22 +3351,22 @@
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>104</v>
+        <v>86</v>
       </c>
       <c r="B98" t="s">
         <v>7</v>
       </c>
       <c r="C98" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D98" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E98" t="s">
-        <v>200</v>
+        <v>174</v>
       </c>
       <c r="F98" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G98">
         <v>150</v>
@@ -3257,24 +3374,668 @@
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="B99" t="s">
         <v>7</v>
       </c>
       <c r="C99" t="s">
+        <v>200</v>
+      </c>
+      <c r="D99" t="s">
+        <v>15</v>
+      </c>
+      <c r="E99" t="s">
+        <v>173</v>
+      </c>
+      <c r="F99" t="s">
+        <v>15</v>
+      </c>
+      <c r="G99">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>87</v>
+      </c>
+      <c r="B100" t="s">
+        <v>7</v>
+      </c>
+      <c r="C100" t="s">
+        <v>200</v>
+      </c>
+      <c r="D100" t="s">
+        <v>15</v>
+      </c>
+      <c r="E100" t="s">
+        <v>175</v>
+      </c>
+      <c r="F100" t="s">
+        <v>15</v>
+      </c>
+      <c r="G100">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>216</v>
+      </c>
+      <c r="B101" t="s">
+        <v>7</v>
+      </c>
+      <c r="C101" t="s">
+        <v>200</v>
+      </c>
+      <c r="D101" t="s">
+        <v>15</v>
+      </c>
+      <c r="E101" t="s">
+        <v>239</v>
+      </c>
+      <c r="F101" t="s">
+        <v>15</v>
+      </c>
+      <c r="G101">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>89</v>
+      </c>
+      <c r="B102" t="s">
+        <v>7</v>
+      </c>
+      <c r="C102" t="s">
+        <v>200</v>
+      </c>
+      <c r="D102" t="s">
+        <v>15</v>
+      </c>
+      <c r="E102" t="s">
+        <v>177</v>
+      </c>
+      <c r="F102" t="s">
+        <v>15</v>
+      </c>
+      <c r="G102">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>94</v>
+      </c>
+      <c r="B103" t="s">
+        <v>7</v>
+      </c>
+      <c r="C103" t="s">
+        <v>200</v>
+      </c>
+      <c r="D103" t="s">
+        <v>15</v>
+      </c>
+      <c r="E103" t="s">
+        <v>184</v>
+      </c>
+      <c r="F103" t="s">
+        <v>15</v>
+      </c>
+      <c r="G103">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>90</v>
+      </c>
+      <c r="B104" t="s">
+        <v>7</v>
+      </c>
+      <c r="C104" t="s">
+        <v>200</v>
+      </c>
+      <c r="D104" t="s">
+        <v>15</v>
+      </c>
+      <c r="E104" t="s">
+        <v>178</v>
+      </c>
+      <c r="F104" t="s">
+        <v>15</v>
+      </c>
+      <c r="G104">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>92</v>
+      </c>
+      <c r="B105" t="s">
+        <v>7</v>
+      </c>
+      <c r="C105" t="s">
+        <v>200</v>
+      </c>
+      <c r="D105" t="s">
+        <v>15</v>
+      </c>
+      <c r="E105" t="s">
+        <v>181</v>
+      </c>
+      <c r="F105" t="s">
+        <v>15</v>
+      </c>
+      <c r="G105">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>71</v>
+      </c>
+      <c r="B106" t="s">
+        <v>7</v>
+      </c>
+      <c r="C106" t="s">
+        <v>200</v>
+      </c>
+      <c r="D106" t="s">
+        <v>15</v>
+      </c>
+      <c r="E106" t="s">
+        <v>159</v>
+      </c>
+      <c r="F106" t="s">
+        <v>15</v>
+      </c>
+      <c r="G106">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>217</v>
+      </c>
+      <c r="B107" t="s">
+        <v>7</v>
+      </c>
+      <c r="C107" t="s">
+        <v>200</v>
+      </c>
+      <c r="D107" t="s">
+        <v>15</v>
+      </c>
+      <c r="E107" t="s">
+        <v>240</v>
+      </c>
+      <c r="F107" t="s">
+        <v>15</v>
+      </c>
+      <c r="G107">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
         <v>202</v>
       </c>
-      <c r="D99" t="s">
-        <v>16</v>
-      </c>
-      <c r="E99" t="s">
-        <v>201</v>
-      </c>
-      <c r="F99" t="s">
-        <v>16</v>
-      </c>
-      <c r="G99">
+      <c r="B108" t="s">
+        <v>7</v>
+      </c>
+      <c r="C108" t="s">
+        <v>200</v>
+      </c>
+      <c r="D108" t="s">
+        <v>15</v>
+      </c>
+      <c r="E108" t="s">
+        <v>179</v>
+      </c>
+      <c r="F108" t="s">
+        <v>15</v>
+      </c>
+      <c r="G108">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>91</v>
+      </c>
+      <c r="B109" t="s">
+        <v>7</v>
+      </c>
+      <c r="C109" t="s">
+        <v>200</v>
+      </c>
+      <c r="D109" t="s">
+        <v>15</v>
+      </c>
+      <c r="E109" t="s">
+        <v>180</v>
+      </c>
+      <c r="F109" t="s">
+        <v>15</v>
+      </c>
+      <c r="G109">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>45</v>
+      </c>
+      <c r="B110" t="s">
+        <v>7</v>
+      </c>
+      <c r="C110" t="s">
+        <v>200</v>
+      </c>
+      <c r="D110" t="s">
+        <v>15</v>
+      </c>
+      <c r="E110" t="s">
+        <v>132</v>
+      </c>
+      <c r="F110" t="s">
+        <v>15</v>
+      </c>
+      <c r="G110">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>93</v>
+      </c>
+      <c r="B111" t="s">
+        <v>7</v>
+      </c>
+      <c r="C111" t="s">
+        <v>200</v>
+      </c>
+      <c r="D111" t="s">
+        <v>15</v>
+      </c>
+      <c r="E111" t="s">
+        <v>183</v>
+      </c>
+      <c r="F111" t="s">
+        <v>15</v>
+      </c>
+      <c r="G111">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>65</v>
+      </c>
+      <c r="B112" t="s">
+        <v>7</v>
+      </c>
+      <c r="C112" t="s">
+        <v>200</v>
+      </c>
+      <c r="D112" t="s">
+        <v>15</v>
+      </c>
+      <c r="E112" t="s">
+        <v>153</v>
+      </c>
+      <c r="F112" t="s">
+        <v>15</v>
+      </c>
+      <c r="G112">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>65</v>
+      </c>
+      <c r="B113" t="s">
+        <v>7</v>
+      </c>
+      <c r="C113" t="s">
+        <v>200</v>
+      </c>
+      <c r="D113" t="s">
+        <v>15</v>
+      </c>
+      <c r="E113" t="s">
+        <v>241</v>
+      </c>
+      <c r="F113" t="s">
+        <v>15</v>
+      </c>
+      <c r="G113">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>96</v>
+      </c>
+      <c r="B114" t="s">
+        <v>7</v>
+      </c>
+      <c r="C114" t="s">
+        <v>200</v>
+      </c>
+      <c r="D114" t="s">
+        <v>15</v>
+      </c>
+      <c r="E114" t="s">
+        <v>186</v>
+      </c>
+      <c r="F114" t="s">
+        <v>15</v>
+      </c>
+      <c r="G114">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>97</v>
+      </c>
+      <c r="B115" t="s">
+        <v>7</v>
+      </c>
+      <c r="C115" t="s">
+        <v>200</v>
+      </c>
+      <c r="D115" t="s">
+        <v>15</v>
+      </c>
+      <c r="E115" t="s">
+        <v>187</v>
+      </c>
+      <c r="F115" t="s">
+        <v>15</v>
+      </c>
+      <c r="G115">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>95</v>
+      </c>
+      <c r="B116" t="s">
+        <v>7</v>
+      </c>
+      <c r="C116" t="s">
+        <v>200</v>
+      </c>
+      <c r="D116" t="s">
+        <v>15</v>
+      </c>
+      <c r="E116" t="s">
+        <v>185</v>
+      </c>
+      <c r="F116" t="s">
+        <v>15</v>
+      </c>
+      <c r="G116">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>95</v>
+      </c>
+      <c r="B117" t="s">
+        <v>7</v>
+      </c>
+      <c r="C117" t="s">
+        <v>200</v>
+      </c>
+      <c r="D117" t="s">
+        <v>15</v>
+      </c>
+      <c r="E117" t="s">
+        <v>242</v>
+      </c>
+      <c r="F117" t="s">
+        <v>15</v>
+      </c>
+      <c r="G117">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>98</v>
+      </c>
+      <c r="B118" t="s">
+        <v>7</v>
+      </c>
+      <c r="C118" t="s">
+        <v>200</v>
+      </c>
+      <c r="D118" t="s">
+        <v>15</v>
+      </c>
+      <c r="E118" t="s">
+        <v>189</v>
+      </c>
+      <c r="F118" t="s">
+        <v>15</v>
+      </c>
+      <c r="G118">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>100</v>
+      </c>
+      <c r="B119" t="s">
+        <v>7</v>
+      </c>
+      <c r="C119" t="s">
+        <v>200</v>
+      </c>
+      <c r="D119" t="s">
+        <v>15</v>
+      </c>
+      <c r="E119" t="s">
+        <v>193</v>
+      </c>
+      <c r="F119" t="s">
+        <v>15</v>
+      </c>
+      <c r="G119">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>61</v>
+      </c>
+      <c r="B120" t="s">
+        <v>7</v>
+      </c>
+      <c r="C120" t="s">
+        <v>200</v>
+      </c>
+      <c r="D120" t="s">
+        <v>15</v>
+      </c>
+      <c r="E120" t="s">
+        <v>148</v>
+      </c>
+      <c r="F120" t="s">
+        <v>15</v>
+      </c>
+      <c r="G120">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>61</v>
+      </c>
+      <c r="B121" t="s">
+        <v>7</v>
+      </c>
+      <c r="C121" t="s">
+        <v>200</v>
+      </c>
+      <c r="D121" t="s">
+        <v>15</v>
+      </c>
+      <c r="E121" t="s">
+        <v>243</v>
+      </c>
+      <c r="F121" t="s">
+        <v>15</v>
+      </c>
+      <c r="G121">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>61</v>
+      </c>
+      <c r="B122" t="s">
+        <v>7</v>
+      </c>
+      <c r="C122" t="s">
+        <v>200</v>
+      </c>
+      <c r="D122" t="s">
+        <v>15</v>
+      </c>
+      <c r="E122" t="s">
+        <v>244</v>
+      </c>
+      <c r="F122" t="s">
+        <v>15</v>
+      </c>
+      <c r="G122">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>61</v>
+      </c>
+      <c r="B123" t="s">
+        <v>7</v>
+      </c>
+      <c r="C123" t="s">
+        <v>200</v>
+      </c>
+      <c r="D123" t="s">
+        <v>15</v>
+      </c>
+      <c r="E123" t="s">
+        <v>191</v>
+      </c>
+      <c r="F123" t="s">
+        <v>15</v>
+      </c>
+      <c r="G123">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>99</v>
+      </c>
+      <c r="B124" t="s">
+        <v>7</v>
+      </c>
+      <c r="C124" t="s">
+        <v>200</v>
+      </c>
+      <c r="D124" t="s">
+        <v>15</v>
+      </c>
+      <c r="E124" t="s">
+        <v>245</v>
+      </c>
+      <c r="F124" t="s">
+        <v>15</v>
+      </c>
+      <c r="G124">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>99</v>
+      </c>
+      <c r="B125" t="s">
+        <v>7</v>
+      </c>
+      <c r="C125" t="s">
+        <v>200</v>
+      </c>
+      <c r="D125" t="s">
+        <v>15</v>
+      </c>
+      <c r="E125" t="s">
+        <v>192</v>
+      </c>
+      <c r="F125" t="s">
+        <v>15</v>
+      </c>
+      <c r="G125">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>102</v>
+      </c>
+      <c r="B126" t="s">
+        <v>7</v>
+      </c>
+      <c r="C126" t="s">
+        <v>200</v>
+      </c>
+      <c r="D126" t="s">
+        <v>15</v>
+      </c>
+      <c r="E126" t="s">
+        <v>198</v>
+      </c>
+      <c r="F126" t="s">
+        <v>15</v>
+      </c>
+      <c r="G126">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>103</v>
+      </c>
+      <c r="B127" t="s">
+        <v>7</v>
+      </c>
+      <c r="C127" t="s">
+        <v>200</v>
+      </c>
+      <c r="D127" t="s">
+        <v>15</v>
+      </c>
+      <c r="E127" t="s">
+        <v>199</v>
+      </c>
+      <c r="F127" t="s">
+        <v>15</v>
+      </c>
+      <c r="G127">
         <v>150</v>
       </c>
     </row>
@@ -3297,12 +4058,12 @@
   <sheetData>
     <row r="1" spans="1:1" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>207</v>
+        <v>246</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
filter price max fix / version
Max price was set below highest price for some items in NHL. Was
preventing them from showing up in standard infinite list.
Changed max price to over double highest item to compensate.
</commit_message>
<xml_diff>
--- a/filters/db/Brands.xlsx
+++ b/filters/db/Brands.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="375" windowWidth="19875" windowHeight="8235" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="375" windowWidth="19875" windowHeight="8235"/>
   </bookViews>
   <sheets>
     <sheet name="Brands" sheetId="1" r:id="rId1"/>
@@ -1112,8 +1112,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G127"/>
   <sheetViews>
-    <sheetView topLeftCell="A101" workbookViewId="0">
-      <selection activeCell="A124" sqref="A124"/>
+    <sheetView tabSelected="1" topLeftCell="E107" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4:G127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1207,7 +1207,7 @@
         <v>15</v>
       </c>
       <c r="G4">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1230,7 +1230,7 @@
         <v>15</v>
       </c>
       <c r="G5">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1253,7 +1253,7 @@
         <v>15</v>
       </c>
       <c r="G6">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1276,7 +1276,7 @@
         <v>15</v>
       </c>
       <c r="G7">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1299,7 +1299,7 @@
         <v>15</v>
       </c>
       <c r="G8">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1322,7 +1322,7 @@
         <v>15</v>
       </c>
       <c r="G9">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1345,7 +1345,7 @@
         <v>15</v>
       </c>
       <c r="G10">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1368,7 +1368,7 @@
         <v>15</v>
       </c>
       <c r="G11">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1391,7 +1391,7 @@
         <v>15</v>
       </c>
       <c r="G12">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1414,7 +1414,7 @@
         <v>15</v>
       </c>
       <c r="G13">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1437,7 +1437,7 @@
         <v>15</v>
       </c>
       <c r="G14">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -1460,7 +1460,7 @@
         <v>15</v>
       </c>
       <c r="G15">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1483,7 +1483,7 @@
         <v>15</v>
       </c>
       <c r="G16">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1506,7 +1506,7 @@
         <v>15</v>
       </c>
       <c r="G17">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1529,7 +1529,7 @@
         <v>15</v>
       </c>
       <c r="G18">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1552,7 +1552,7 @@
         <v>15</v>
       </c>
       <c r="G19">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1575,7 +1575,7 @@
         <v>15</v>
       </c>
       <c r="G20">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1598,7 +1598,7 @@
         <v>15</v>
       </c>
       <c r="G21">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1621,7 +1621,7 @@
         <v>15</v>
       </c>
       <c r="G22">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1644,7 +1644,7 @@
         <v>15</v>
       </c>
       <c r="G23">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1667,7 +1667,7 @@
         <v>15</v>
       </c>
       <c r="G24">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1690,7 +1690,7 @@
         <v>15</v>
       </c>
       <c r="G25">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1713,7 +1713,7 @@
         <v>15</v>
       </c>
       <c r="G26">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1736,7 +1736,7 @@
         <v>15</v>
       </c>
       <c r="G27">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1759,7 +1759,7 @@
         <v>15</v>
       </c>
       <c r="G28">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1782,7 +1782,7 @@
         <v>15</v>
       </c>
       <c r="G29">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -1805,7 +1805,7 @@
         <v>15</v>
       </c>
       <c r="G30">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -1828,7 +1828,7 @@
         <v>15</v>
       </c>
       <c r="G31">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -1851,7 +1851,7 @@
         <v>15</v>
       </c>
       <c r="G32">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -1874,7 +1874,7 @@
         <v>15</v>
       </c>
       <c r="G33">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -1897,7 +1897,7 @@
         <v>15</v>
       </c>
       <c r="G34">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -1920,7 +1920,7 @@
         <v>15</v>
       </c>
       <c r="G35">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -1943,7 +1943,7 @@
         <v>15</v>
       </c>
       <c r="G36">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -1966,7 +1966,7 @@
         <v>15</v>
       </c>
       <c r="G37">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -1989,7 +1989,7 @@
         <v>15</v>
       </c>
       <c r="G38">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -2012,7 +2012,7 @@
         <v>15</v>
       </c>
       <c r="G39">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -2035,7 +2035,7 @@
         <v>15</v>
       </c>
       <c r="G40">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -2058,7 +2058,7 @@
         <v>15</v>
       </c>
       <c r="G41">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -2081,7 +2081,7 @@
         <v>15</v>
       </c>
       <c r="G42">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -2104,7 +2104,7 @@
         <v>15</v>
       </c>
       <c r="G43">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -2127,7 +2127,7 @@
         <v>15</v>
       </c>
       <c r="G44">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -2150,7 +2150,7 @@
         <v>15</v>
       </c>
       <c r="G45">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -2173,7 +2173,7 @@
         <v>15</v>
       </c>
       <c r="G46">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -2196,7 +2196,7 @@
         <v>15</v>
       </c>
       <c r="G47">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -2219,7 +2219,7 @@
         <v>15</v>
       </c>
       <c r="G48">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -2242,7 +2242,7 @@
         <v>15</v>
       </c>
       <c r="G49">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -2265,7 +2265,7 @@
         <v>15</v>
       </c>
       <c r="G50">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
@@ -2288,7 +2288,7 @@
         <v>15</v>
       </c>
       <c r="G51">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -2311,7 +2311,7 @@
         <v>15</v>
       </c>
       <c r="G52">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -2334,7 +2334,7 @@
         <v>15</v>
       </c>
       <c r="G53">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -2357,7 +2357,7 @@
         <v>15</v>
       </c>
       <c r="G54">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -2380,7 +2380,7 @@
         <v>15</v>
       </c>
       <c r="G55">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
@@ -2403,7 +2403,7 @@
         <v>15</v>
       </c>
       <c r="G56">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
@@ -2426,7 +2426,7 @@
         <v>15</v>
       </c>
       <c r="G57">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
@@ -2449,7 +2449,7 @@
         <v>15</v>
       </c>
       <c r="G58">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
@@ -2472,7 +2472,7 @@
         <v>15</v>
       </c>
       <c r="G59">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
@@ -2495,7 +2495,7 @@
         <v>15</v>
       </c>
       <c r="G60">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
@@ -2518,7 +2518,7 @@
         <v>15</v>
       </c>
       <c r="G61">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
@@ -2541,7 +2541,7 @@
         <v>15</v>
       </c>
       <c r="G62">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
@@ -2564,7 +2564,7 @@
         <v>15</v>
       </c>
       <c r="G63">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
@@ -2587,7 +2587,7 @@
         <v>15</v>
       </c>
       <c r="G64">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
@@ -2610,7 +2610,7 @@
         <v>15</v>
       </c>
       <c r="G65">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
@@ -2633,7 +2633,7 @@
         <v>15</v>
       </c>
       <c r="G66">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
@@ -2656,7 +2656,7 @@
         <v>15</v>
       </c>
       <c r="G67">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
@@ -2679,7 +2679,7 @@
         <v>15</v>
       </c>
       <c r="G68">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
@@ -2702,7 +2702,7 @@
         <v>15</v>
       </c>
       <c r="G69">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
@@ -2725,7 +2725,7 @@
         <v>15</v>
       </c>
       <c r="G70">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
@@ -2748,7 +2748,7 @@
         <v>15</v>
       </c>
       <c r="G71">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
@@ -2771,7 +2771,7 @@
         <v>15</v>
       </c>
       <c r="G72">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
@@ -2794,7 +2794,7 @@
         <v>15</v>
       </c>
       <c r="G73">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
@@ -2817,7 +2817,7 @@
         <v>15</v>
       </c>
       <c r="G74">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
@@ -2840,7 +2840,7 @@
         <v>15</v>
       </c>
       <c r="G75">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
@@ -2863,7 +2863,7 @@
         <v>15</v>
       </c>
       <c r="G76">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
@@ -2886,7 +2886,7 @@
         <v>15</v>
       </c>
       <c r="G77">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
@@ -2909,7 +2909,7 @@
         <v>15</v>
       </c>
       <c r="G78">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
@@ -2932,7 +2932,7 @@
         <v>15</v>
       </c>
       <c r="G79">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
@@ -2955,7 +2955,7 @@
         <v>15</v>
       </c>
       <c r="G80">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
@@ -2978,7 +2978,7 @@
         <v>15</v>
       </c>
       <c r="G81">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
@@ -3001,7 +3001,7 @@
         <v>15</v>
       </c>
       <c r="G82">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
@@ -3024,7 +3024,7 @@
         <v>15</v>
       </c>
       <c r="G83">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
@@ -3047,7 +3047,7 @@
         <v>15</v>
       </c>
       <c r="G84">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
@@ -3070,7 +3070,7 @@
         <v>15</v>
       </c>
       <c r="G85">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
@@ -3093,7 +3093,7 @@
         <v>15</v>
       </c>
       <c r="G86">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
@@ -3116,7 +3116,7 @@
         <v>15</v>
       </c>
       <c r="G87">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
@@ -3139,7 +3139,7 @@
         <v>15</v>
       </c>
       <c r="G88">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
@@ -3162,7 +3162,7 @@
         <v>15</v>
       </c>
       <c r="G89">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
@@ -3185,7 +3185,7 @@
         <v>15</v>
       </c>
       <c r="G90">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
@@ -3208,7 +3208,7 @@
         <v>15</v>
       </c>
       <c r="G91">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
@@ -3231,7 +3231,7 @@
         <v>15</v>
       </c>
       <c r="G92">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
@@ -3254,7 +3254,7 @@
         <v>15</v>
       </c>
       <c r="G93">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
@@ -3277,7 +3277,7 @@
         <v>15</v>
       </c>
       <c r="G94">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
@@ -3300,7 +3300,7 @@
         <v>15</v>
       </c>
       <c r="G95">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
@@ -3323,7 +3323,7 @@
         <v>15</v>
       </c>
       <c r="G96">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
@@ -3346,7 +3346,7 @@
         <v>15</v>
       </c>
       <c r="G97">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
@@ -3369,7 +3369,7 @@
         <v>15</v>
       </c>
       <c r="G98">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
@@ -3392,7 +3392,7 @@
         <v>15</v>
       </c>
       <c r="G99">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
@@ -3415,7 +3415,7 @@
         <v>15</v>
       </c>
       <c r="G100">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
@@ -3438,7 +3438,7 @@
         <v>15</v>
       </c>
       <c r="G101">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
@@ -3461,7 +3461,7 @@
         <v>15</v>
       </c>
       <c r="G102">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
@@ -3484,7 +3484,7 @@
         <v>15</v>
       </c>
       <c r="G103">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
@@ -3507,7 +3507,7 @@
         <v>15</v>
       </c>
       <c r="G104">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
@@ -3530,7 +3530,7 @@
         <v>15</v>
       </c>
       <c r="G105">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
@@ -3553,7 +3553,7 @@
         <v>15</v>
       </c>
       <c r="G106">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
@@ -3576,7 +3576,7 @@
         <v>15</v>
       </c>
       <c r="G107">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
@@ -3599,7 +3599,7 @@
         <v>15</v>
       </c>
       <c r="G108">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
@@ -3622,7 +3622,7 @@
         <v>15</v>
       </c>
       <c r="G109">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
@@ -3645,7 +3645,7 @@
         <v>15</v>
       </c>
       <c r="G110">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
@@ -3668,7 +3668,7 @@
         <v>15</v>
       </c>
       <c r="G111">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
@@ -3691,7 +3691,7 @@
         <v>15</v>
       </c>
       <c r="G112">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
@@ -3714,7 +3714,7 @@
         <v>15</v>
       </c>
       <c r="G113">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
@@ -3737,7 +3737,7 @@
         <v>15</v>
       </c>
       <c r="G114">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
@@ -3760,7 +3760,7 @@
         <v>15</v>
       </c>
       <c r="G115">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
@@ -3783,7 +3783,7 @@
         <v>15</v>
       </c>
       <c r="G116">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
@@ -3806,7 +3806,7 @@
         <v>15</v>
       </c>
       <c r="G117">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
@@ -3829,7 +3829,7 @@
         <v>15</v>
       </c>
       <c r="G118">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
@@ -3852,7 +3852,7 @@
         <v>15</v>
       </c>
       <c r="G119">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
@@ -3875,7 +3875,7 @@
         <v>15</v>
       </c>
       <c r="G120">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
@@ -3898,7 +3898,7 @@
         <v>15</v>
       </c>
       <c r="G121">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
@@ -3921,7 +3921,7 @@
         <v>15</v>
       </c>
       <c r="G122">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
@@ -3944,7 +3944,7 @@
         <v>15</v>
       </c>
       <c r="G123">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
@@ -3967,7 +3967,7 @@
         <v>15</v>
       </c>
       <c r="G124">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
@@ -3990,7 +3990,7 @@
         <v>15</v>
       </c>
       <c r="G125">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
@@ -4013,7 +4013,7 @@
         <v>15</v>
       </c>
       <c r="G126">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
@@ -4036,7 +4036,7 @@
         <v>15</v>
       </c>
       <c r="G127">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
   </sheetData>
@@ -4049,7 +4049,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>